<commit_message>
Successfuly Tested Bastion Host Deployment
</commit_message>
<xml_diff>
--- a/aws_terraform/deployments/bastion_host/Terraform BastionHost.xlsx
+++ b/aws_terraform/deployments/bastion_host/Terraform BastionHost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfroggatt/Desktop/git/Personal/AWS-Automation/aws_terraform/deployments/bastion_host/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F805853B-3E55-7A4E-8D80-606E0CDE77CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED88B3A-C0DA-0A45-B021-3DACC8EE30FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1540" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>VariableName</t>
   </si>
@@ -87,9 +87,6 @@
     <t>****************************************</t>
   </si>
   <si>
-    <t>us-east-2</t>
-  </si>
-  <si>
     <t>The AWS Region</t>
   </si>
   <si>
@@ -111,15 +108,6 @@
     <t>The vpc id to deploy the instances in to</t>
   </si>
   <si>
-    <t>86.7.1.174</t>
-  </si>
-  <si>
-    <t>vpc-xxxxxxxx</t>
-  </si>
-  <si>
-    <t>subnet-xxxxxxxx</t>
-  </si>
-  <si>
     <t>The name of the EC2 instance key to use</t>
   </si>
   <si>
@@ -135,13 +123,28 @@
     <t>Management</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>t3.nano</t>
   </si>
   <si>
     <t>The ec2 instance size</t>
+  </si>
+  <si>
+    <t>vpc-14ee357d</t>
+  </si>
+  <si>
+    <t>212.139.37.214</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Ryan Froggatt</t>
+  </si>
+  <si>
+    <t>eu-west-2</t>
+  </si>
+  <si>
+    <t>subnet-6831fd13</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1038,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,7 +1074,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1085,7 +1088,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1093,13 +1096,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1107,13 +1110,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1121,13 +1124,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1135,13 +1138,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1149,13 +1152,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1163,13 +1166,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1177,25 +1180,27 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1203,13 +1208,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1217,13 +1222,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>